<commit_message>
in the session(user_id data type is varchar)but in the user(user_id data type is int).is it correct?
</commit_message>
<xml_diff>
--- a/IMS_Documents/IMS Data Model.xlsx
+++ b/IMS_Documents/IMS Data Model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="91">
   <si>
     <t>Column Name</t>
   </si>
@@ -283,19 +283,10 @@
     <t>FK(Item_Category: Item_Category_ID)</t>
   </si>
   <si>
-    <t>FK(Item_Company:Item_Company_ID)</t>
-  </si>
-  <si>
-    <t>Item_Model(FK:Item_Category_ID)</t>
-  </si>
-  <si>
-    <t>Item_Model(FK:Item_Company_ID)</t>
-  </si>
-  <si>
-    <t>Item_Model(FK:Item_Model_ID)</t>
-  </si>
-  <si>
-    <t>Item_Model(FK:Item_ID)</t>
+    <t>FK(Company:Item_Company_ID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -448,10 +439,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,7 +540,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -760,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:G54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,20 +772,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -990,13 +981,13 @@
         <v>35</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
@@ -1091,13 +1082,13 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
       <c r="J15" s="1">
         <v>4</v>
       </c>
@@ -1288,6 +1279,11 @@
       </c>
       <c r="G23" s="1" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
@@ -1410,11 +1406,19 @@
       <c r="G33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="1"/>
+      <c r="J33" s="1">
+        <v>3</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
@@ -1975,7 +1979,7 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
-      <c r="G57" s="11"/>
+      <c r="G57" s="12"/>
       <c r="J57" s="1">
         <v>11</v>
       </c>
@@ -2066,7 +2070,7 @@
         <v>35</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="J60" s="1">
         <v>14</v>
@@ -2096,7 +2100,7 @@
         <v>35</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="J61" s="1">
         <v>15</v>
@@ -2126,7 +2130,7 @@
         <v>35</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="3:14" x14ac:dyDescent="0.25">
@@ -2143,7 +2147,7 @@
         <v>35</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="J63" s="10" t="s">
         <v>31</v>
@@ -2374,7 +2378,7 @@
       <c r="D72" s="10"/>
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
-      <c r="G72" s="11"/>
+      <c r="G72" s="12"/>
       <c r="J72" s="1">
         <v>8</v>
       </c>
@@ -2694,13 +2698,13 @@
       </c>
     </row>
     <row r="90" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C90" s="12" t="s">
+      <c r="C90" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
     </row>
     <row r="91" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C91" s="2" t="s">
@@ -2860,6 +2864,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="J63:N63"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="J78:N78"/>
     <mergeCell ref="J42:N42"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="J2:N2"/>
@@ -2868,11 +2877,6 @@
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="J29:N29"/>
     <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="J63:N63"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="J78:N78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>